<commit_message>
added new furnace valve connections
added new furnace valve connections
valve actuation and position
</commit_message>
<xml_diff>
--- a/furnace/furnace.connections.2016.xlsx
+++ b/furnace/furnace.connections.2016.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="112">
   <si>
     <t>0 V</t>
   </si>
@@ -147,9 +147,6 @@
     <t xml:space="preserve">25 pin DB25 cable furnace to e-box </t>
   </si>
   <si>
-    <t>blue x 3</t>
-  </si>
-  <si>
     <t>Standalone furnace extraction system connections 1/29/16</t>
   </si>
   <si>
@@ -297,18 +294,6 @@
     <t>nc</t>
   </si>
   <si>
-    <t>brown x 3 + red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 V </t>
-  </si>
-  <si>
-    <t>H2O power</t>
-  </si>
-  <si>
-    <t>to be changed</t>
-  </si>
-  <si>
     <t>H2O OK</t>
   </si>
   <si>
@@ -318,10 +303,58 @@
     <t>output 24 V</t>
   </si>
   <si>
-    <t>add 24 V to H2O</t>
-  </si>
-  <si>
-    <t>add H2O ground</t>
+    <t>9 pin connector</t>
+  </si>
+  <si>
+    <t>0 V - solenoid ground</t>
+  </si>
+  <si>
+    <t>manual switches</t>
+  </si>
+  <si>
+    <t>12 V</t>
+  </si>
+  <si>
+    <t>ground terminal block</t>
+  </si>
+  <si>
+    <t>24 V terminal block</t>
+  </si>
+  <si>
+    <t>H2O  sensor power</t>
+  </si>
+  <si>
+    <t>furnace open switch</t>
+  </si>
+  <si>
+    <t>rough turbo valve</t>
+  </si>
+  <si>
+    <t>getter  valve</t>
+  </si>
+  <si>
+    <t>rough valve</t>
+  </si>
+  <si>
+    <t>furnace turbo valve</t>
+  </si>
+  <si>
+    <t>lower shutter actuate</t>
+  </si>
+  <si>
+    <t>upper shutter actuate</t>
+  </si>
+  <si>
+    <t>furnace valve</t>
+  </si>
+  <si>
+    <t>signal terminal block</t>
+  </si>
+  <si>
+    <t>gate  valve</t>
+  </si>
+  <si>
+    <t>getter valve</t>
   </si>
 </sst>
 </file>
@@ -391,8 +424,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="217">
+  <cellStyleXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -615,7 +658,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="217">
+  <cellStyles count="227">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -724,6 +767,11 @@
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -832,6 +880,11 @@
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1164,20 +1217,19 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G85"/>
+  <dimension ref="A2:G97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="6" width="18.5" customWidth="1"/>
-    <col min="7" max="7" width="10.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
+    <col min="4" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" customWidth="1"/>
     <col min="8" max="8" width="3.1640625" customWidth="1"/>
     <col min="9" max="9" width="4.1640625" customWidth="1"/>
     <col min="14" max="14" width="26" customWidth="1"/>
@@ -1185,31 +1237,31 @@
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="B5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="C8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1220,7 +1272,7 @@
         <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9">
         <v>1</v>
@@ -1237,7 +1289,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10">
         <v>2</v>
@@ -1254,7 +1306,7 @@
         <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1271,7 +1323,7 @@
         <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <v>4</v>
@@ -1288,7 +1340,7 @@
         <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -1305,7 +1357,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D14">
         <v>6</v>
@@ -1322,10 +1374,10 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1333,13 +1385,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1347,13 +1399,13 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1361,21 +1413,21 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="B21" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1383,13 +1435,13 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E23">
         <v>16</v>
@@ -1403,10 +1455,10 @@
         <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E24">
         <v>17</v>
@@ -1420,10 +1472,10 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E25">
         <v>18</v>
@@ -1437,10 +1489,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E26">
         <v>2</v>
@@ -1454,10 +1506,10 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E27">
         <v>3</v>
@@ -1471,10 +1523,10 @@
         <v>22</v>
       </c>
       <c r="C28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E28">
         <v>4</v>
@@ -1488,10 +1540,10 @@
         <v>22</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E29">
         <v>5</v>
@@ -1505,10 +1557,10 @@
         <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E30">
         <v>6</v>
@@ -1522,510 +1574,651 @@
         <v>20</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E31">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:5">
       <c r="B34" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="C36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38">
+        <v>3</v>
+      </c>
+      <c r="B38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40">
+        <v>5</v>
+      </c>
+      <c r="B40" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>110</v>
+      </c>
+      <c r="C42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43">
+        <v>8</v>
+      </c>
+      <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44">
+        <v>9</v>
+      </c>
+      <c r="B44" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="B46" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="B47" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="B35" t="s">
+      <c r="C47" t="s">
         <v>57</v>
       </c>
-      <c r="C35" t="s">
+    </row>
+    <row r="48" spans="1:5">
+      <c r="B48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="B36" t="s">
+    <row r="49" spans="1:7">
+      <c r="C49" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="C37" t="s">
+    <row r="51" spans="1:7">
+      <c r="C51" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
-      <c r="C39" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7">
-      <c r="B42" s="2" t="s">
+    <row r="54" spans="1:7">
+      <c r="B54" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
-      <c r="B43" s="2"/>
-      <c r="E43" t="s">
+    <row r="55" spans="1:7">
+      <c r="B55" s="2"/>
+      <c r="E55" t="s">
+        <v>74</v>
+      </c>
+      <c r="F55" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" t="s">
         <v>75</v>
-      </c>
-      <c r="G43" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>0</v>
-      </c>
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
-      <c r="G44" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45">
-        <v>2</v>
-      </c>
-      <c r="B45" t="s">
-        <v>97</v>
-      </c>
-      <c r="C45" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7">
-      <c r="A46">
-        <v>3</v>
-      </c>
-      <c r="B46" t="s">
-        <v>97</v>
-      </c>
-      <c r="C46" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47">
-        <v>4</v>
-      </c>
-      <c r="B47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7">
-      <c r="A48">
-        <v>5</v>
-      </c>
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49">
-        <v>6</v>
-      </c>
-      <c r="B49" t="s">
-        <v>97</v>
-      </c>
-      <c r="C49" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50">
-        <v>7</v>
-      </c>
-      <c r="B50" t="s">
-        <v>97</v>
-      </c>
-      <c r="C50" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7">
-      <c r="A51">
-        <v>8</v>
-      </c>
-      <c r="B51" t="s">
-        <v>0</v>
-      </c>
-      <c r="C51" t="s">
-        <v>31</v>
-      </c>
-      <c r="E51" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7">
-      <c r="A52">
-        <v>9</v>
-      </c>
-      <c r="B52" t="s">
-        <v>32</v>
-      </c>
-      <c r="C52" t="s">
-        <v>33</v>
-      </c>
-      <c r="E52" t="s">
-        <v>92</v>
-      </c>
-      <c r="F52" t="s">
-        <v>99</v>
-      </c>
-      <c r="G52" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53">
-        <v>10</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1"/>
-      <c r="E53" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
-      <c r="A54">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C54" t="s">
-        <v>1</v>
-      </c>
-      <c r="E54" t="s">
-        <v>7</v>
-      </c>
-      <c r="F54" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
-      <c r="A55">
-        <v>12</v>
-      </c>
-      <c r="B55" t="s">
-        <v>98</v>
-      </c>
-      <c r="C55" t="s">
-        <v>2</v>
-      </c>
-      <c r="E55" t="s">
-        <v>8</v>
-      </c>
-      <c r="G55" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>3</v>
-      </c>
-      <c r="E56" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="G56" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="57" spans="1:7">
       <c r="A57">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C57" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="G57" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="58" spans="1:7">
       <c r="A58">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C58" t="s">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="G58" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="B59" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C59" t="s">
-        <v>34</v>
-      </c>
-      <c r="E59" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G59" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="A60">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B60" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C60" t="s">
-        <v>17</v>
-      </c>
-      <c r="E60" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="G60" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
     </row>
     <row r="61" spans="1:7">
       <c r="A61">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C61" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G61" t="s">
-        <v>27</v>
+        <v>109</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="A62">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="B62" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>11</v>
+        <v>37</v>
+      </c>
+      <c r="G62" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="63" spans="1:7">
       <c r="A63">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="B63" t="s">
+        <v>0</v>
+      </c>
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="G63" t="s">
         <v>98</v>
-      </c>
-      <c r="C63" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="64" spans="1:7">
       <c r="A64">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
       <c r="C64" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
+        <v>33</v>
+      </c>
+      <c r="E64" t="s">
+        <v>99</v>
+      </c>
+      <c r="G64" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65">
-        <v>22</v>
-      </c>
-      <c r="B65" t="s">
-        <v>98</v>
-      </c>
-      <c r="C65" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
+        <v>10</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B66" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C66" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B67" t="s">
         <v>93</v>
       </c>
       <c r="C67" t="s">
-        <v>94</v>
-      </c>
-      <c r="F67" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
+        <v>2</v>
+      </c>
+      <c r="E67" t="s">
+        <v>8</v>
+      </c>
+      <c r="G67" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68">
+        <v>13</v>
+      </c>
+      <c r="B68" t="s">
+        <v>93</v>
+      </c>
+      <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="E68" t="s">
+        <v>8</v>
+      </c>
+      <c r="G68" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
+      <c r="A69">
+        <v>14</v>
+      </c>
+      <c r="B69" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
+      </c>
+      <c r="F69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
+      <c r="A70">
+        <v>15</v>
+      </c>
+      <c r="B70" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" t="s">
+        <v>10</v>
+      </c>
+      <c r="F70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
+      <c r="A71">
+        <v>16</v>
+      </c>
+      <c r="B71" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" t="s">
+        <v>40</v>
+      </c>
+      <c r="G71" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
+      <c r="A72">
+        <v>17</v>
+      </c>
+      <c r="B72" t="s">
+        <v>92</v>
+      </c>
+      <c r="C72" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" t="s">
+        <v>28</v>
+      </c>
+      <c r="G72" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
+      <c r="A73">
+        <v>18</v>
+      </c>
+      <c r="B73" t="s">
+        <v>92</v>
+      </c>
+      <c r="C73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>28</v>
+      </c>
+      <c r="G73" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
+      <c r="A74">
+        <v>19</v>
+      </c>
+      <c r="B74" t="s">
+        <v>93</v>
+      </c>
+      <c r="C74" t="s">
+        <v>11</v>
+      </c>
+      <c r="F74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
+      <c r="A75">
+        <v>20</v>
+      </c>
+      <c r="B75" t="s">
+        <v>93</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
+      <c r="A76">
+        <v>21</v>
+      </c>
+      <c r="B76" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" t="s">
+        <v>13</v>
+      </c>
+      <c r="F76" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
+      <c r="A77">
+        <v>22</v>
+      </c>
+      <c r="B77" t="s">
+        <v>93</v>
+      </c>
+      <c r="C77" t="s">
+        <v>14</v>
+      </c>
+      <c r="F77" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
+      <c r="A78">
+        <v>23</v>
+      </c>
+      <c r="B78" t="s">
+        <v>93</v>
+      </c>
+      <c r="C78" t="s">
+        <v>15</v>
+      </c>
+      <c r="F78" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
+      <c r="A79">
+        <v>24</v>
+      </c>
+      <c r="B79" t="s">
+        <v>92</v>
+      </c>
+      <c r="C79" t="s">
+        <v>101</v>
+      </c>
+      <c r="E79" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
+      <c r="A80">
         <v>25</v>
       </c>
-      <c r="B68" t="s">
-        <v>97</v>
-      </c>
-      <c r="C68" t="s">
-        <v>96</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" t="s">
+      <c r="B80" t="s">
+        <v>92</v>
+      </c>
+      <c r="C80" t="s">
+        <v>91</v>
+      </c>
+      <c r="E80" t="s">
+        <v>8</v>
+      </c>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" t="s">
-        <v>85</v>
-      </c>
-      <c r="B79" t="s">
-        <v>88</v>
-      </c>
-      <c r="C79" t="s">
-        <v>86</v>
-      </c>
-      <c r="D79" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6">
-      <c r="A80">
-        <v>1</v>
-      </c>
-      <c r="B80" t="s">
-        <v>32</v>
-      </c>
-      <c r="C80" t="s">
-        <v>80</v>
-      </c>
-      <c r="D80" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81">
-        <v>2</v>
-      </c>
-      <c r="B81" t="s">
-        <v>89</v>
-      </c>
-      <c r="C81" t="s">
-        <v>81</v>
-      </c>
-      <c r="D81" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82">
-        <v>3</v>
-      </c>
-      <c r="B82" t="s">
-        <v>90</v>
-      </c>
-      <c r="C82" t="s">
-        <v>83</v>
-      </c>
-      <c r="D82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83">
-        <v>4</v>
-      </c>
-      <c r="B83" t="s">
-        <v>91</v>
-      </c>
-      <c r="C83" t="s">
-        <v>30</v>
-      </c>
-      <c r="D83" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84">
-        <v>5</v>
-      </c>
-      <c r="B84" t="s">
-        <v>91</v>
-      </c>
-      <c r="C84" t="s">
-        <v>6</v>
-      </c>
-      <c r="D84" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" t="s">
+        <v>84</v>
+      </c>
+      <c r="B91" t="s">
+        <v>87</v>
+      </c>
+      <c r="C91" t="s">
+        <v>85</v>
+      </c>
+      <c r="D91" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92">
+        <v>1</v>
+      </c>
+      <c r="B92" t="s">
+        <v>32</v>
+      </c>
+      <c r="C92" t="s">
+        <v>79</v>
+      </c>
+      <c r="D92" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93">
+        <v>2</v>
+      </c>
+      <c r="B93" t="s">
+        <v>88</v>
+      </c>
+      <c r="C93" t="s">
+        <v>80</v>
+      </c>
+      <c r="D93" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94">
+        <v>3</v>
+      </c>
+      <c r="B94" t="s">
+        <v>89</v>
+      </c>
+      <c r="C94" t="s">
         <v>82</v>
       </c>
-      <c r="B85" t="s">
-        <v>84</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="D94" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95">
+        <v>4</v>
+      </c>
+      <c r="B95" t="s">
+        <v>90</v>
+      </c>
+      <c r="C95" t="s">
+        <v>30</v>
+      </c>
+      <c r="D95" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96">
+        <v>5</v>
+      </c>
+      <c r="B96" t="s">
+        <v>90</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" t="s">
+        <v>81</v>
+      </c>
+      <c r="B97" t="s">
+        <v>83</v>
+      </c>
+      <c r="C97" t="s">
         <v>28</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D97" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup scale="50" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup scale="44" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>